<commit_message>
Carriers: Add P2P US2 calculator, maintenance docs, and reference files
- P2P US2: New carrier module with dual-service calculator (PFA + PFS),
  surcharges, rate extraction, zone mapping (93,100 ZIPs), and upload script
- Add maintenance/logic docs for FedEx, Maersk US, OnTrac, P2P US, USPS
- FedEx: Update 2026 rate card and add supplement contract documents
- USPS: Archive 2025 base rates, add 2026 rate card

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/carriers/fedex/temp_files/Est Picanova Summary 2026.xlsx
+++ b/carriers/fedex/temp_files/Est Picanova Summary 2026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\483935\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\WZQPE24O\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niklavs.felsbergs\Desktop\SHIPPING-COSTS\carriers\fedex\temp_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DC362-EBA4-40CC-8D54-52645342702A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70840464-CBE8-4664-BD9F-D920E58F00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2730" windowWidth="21600" windowHeight="11235" xr2:uid="{AF7DD82B-7C41-4369-AF28-293CE3335E44}"/>
+    <workbookView xWindow="-28920" yWindow="240" windowWidth="29040" windowHeight="15720" xr2:uid="{AF7DD82B-7C41-4369-AF28-293CE3335E44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,10 +174,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +219,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -396,10 +404,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +485,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -490,15 +506,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,31 +844,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DAFC2-3F79-4871-BC82-A5ABDCD1FD9B}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="7" customWidth="1"/>
-    <col min="3" max="5" width="16.28515625" style="8" customWidth="1"/>
-    <col min="9" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="7" customWidth="1"/>
+    <col min="3" max="5" width="16.26953125" style="8" customWidth="1"/>
+    <col min="9" max="10" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -871,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -888,7 +904,7 @@
         <v>-2831.0600000000031</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -905,7 +921,7 @@
         <v>-733.47000000000025</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -922,7 +938,7 @@
         <v>-417.95000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -939,7 +955,7 @@
         <v>-6766.0299999999988</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -956,7 +972,7 @@
         <v>-75.21999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
@@ -973,7 +989,7 @@
         <v>-7167.0300000000116</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>-918566.14000000083</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1023,7 @@
         <v>-4879.6099999999715</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
@@ -1028,8 +1044,8 @@
         <v>-941436.51000000082</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
@@ -1046,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -1066,8 +1082,8 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="7">
@@ -1079,14 +1095,14 @@
       <c r="D15" s="8">
         <v>38457.5</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="27">
         <v>-27689.399999999994</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1122,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1126,7 +1142,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1146,7 +1162,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1184,7 @@
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
@@ -1189,8 +1205,8 @@
         <v>-55789.062000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="20" t="s">
         <v>23</v>
       </c>
@@ -1206,24 +1222,42 @@
         <f>E20+E11</f>
         <v>-997225.57200000086</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="G22">
+        <f>E22/C22</f>
+        <v>-0.33342744938828511</v>
+      </c>
+      <c r="K22" s="35">
+        <v>103398</v>
+      </c>
+      <c r="L22" s="35">
+        <v>147114</v>
+      </c>
+      <c r="M22" s="35">
+        <f>K22-L22</f>
+        <v>-43716</v>
+      </c>
+      <c r="N22" s="34">
+        <f>M22/L22</f>
+        <v>-0.2971573065785717</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-    </row>
-    <row r="25" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +1273,7 @@
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
     </row>
-    <row r="26" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>26</v>
       </c>
@@ -1255,34 +1289,34 @@
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
     </row>
-    <row r="27" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
     </row>
-    <row r="28" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+    <row r="28" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="25"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1292,71 +1326,71 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
       <c r="M31" s="26"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
       <c r="E34"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
       <c r="M34" s="26"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -1366,57 +1400,57 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>

</xml_diff>